<commit_message>
all test are done. Code is ready.
</commit_message>
<xml_diff>
--- a/schedule_1.xlsx
+++ b/schedule_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="168">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -224,6 +224,306 @@
   </si>
   <si>
     <t xml:space="preserve">Vasco DeGama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE lesson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gym Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hercules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michaek Faraday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrico Fermi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shakespeare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alfred Nobel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charles Darwin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie Curie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winston Churchill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euclid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William Shakespeare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English Literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia Woolf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carl Friedrich Gauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dmitri Mendeleev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herodotus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louis Pasteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan Turing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konstantin Stanislavski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Faraday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferdinand Magellan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pablo Picasso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">René Descartes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane Austen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napoleon Bonaparte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usain Bolt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linus Pauling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Tolstoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johann Sebastian Bach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gregor Mendel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immanuel Kant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo da Vinci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonhard Euler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julius Caesar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Clerk Maxwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Orwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antoine Lavoisier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexander von Humboldt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelé</t>
   </si>
 </sst>
 </file>
@@ -362,13 +662,13 @@
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.58"/>
@@ -376,11 +676,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.58"/>
@@ -393,8 +693,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="15.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="17.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="28" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="15.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="16.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="31" style="1" width="11.54"/>
   </cols>
@@ -673,6 +974,558 @@
       </c>
       <c r="AD3" s="4" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="4" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>